<commit_message>
Added time zone offsets for standard and daylight savings
</commit_message>
<xml_diff>
--- a/examples/AtlasGeoTest.xlsx
+++ b/examples/AtlasGeoTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\repos\AtlasGeoAddin\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B43833D-7D6B-4EC9-B3D7-182BB4EFD674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01A2BC2-8F46-4BC4-9E26-1C89B089187B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{1E8F694D-E107-46A2-B946-5E661F5F05A3}"/>
   </bookViews>
@@ -2096,8 +2096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C592D3-75AA-4C40-9417-51BDDD9A314A}">
   <dimension ref="A1:O358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>